<commit_message>
fix: removed extra for
</commit_message>
<xml_diff>
--- a/data/23_05_medfasee_brazil_status_flags.xlsx
+++ b/data/23_05_medfasee_brazil_status_flags.xlsx
@@ -77,7 +77,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -115,11 +115,55 @@
       </bottom>
     </border>
     <border/>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
@@ -184,6 +228,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4885,11 +4941,11 @@
       <c r="E1" s="18" t="n"/>
       <c r="F1" s="18" t="n"/>
       <c r="G1" s="18" t="n"/>
-      <c r="H1" s="19" t="n"/>
-      <c r="I1" s="20" t="n"/>
-      <c r="J1" s="20" t="n"/>
-      <c r="K1" s="20" t="n"/>
-      <c r="L1" s="20" t="n"/>
+      <c r="H1" s="18" t="n"/>
+      <c r="I1" s="18" t="n"/>
+      <c r="J1" s="18" t="n"/>
+      <c r="K1" s="18" t="n"/>
+      <c r="L1" s="18" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="21" t="inlineStr">
@@ -4927,7 +4983,7 @@
           <t>Período</t>
         </is>
       </c>
-      <c r="H2" s="19" t="n"/>
+      <c r="H2" s="20" t="n"/>
       <c r="I2" s="22" t="inlineStr">
         <is>
           <t>Status Flag</t>
@@ -4983,7 +5039,7 @@
           <t>00:00:00.467</t>
         </is>
       </c>
-      <c r="H3" s="19" t="n"/>
+      <c r="H3" s="20" t="n"/>
       <c r="I3" s="21" t="inlineStr">
         <is>
           <t>DE1F0</t>
@@ -5037,7 +5093,7 @@
           <t>00:00:01.116</t>
         </is>
       </c>
-      <c r="H4" s="19" t="n"/>
+      <c r="H4" s="20" t="n"/>
       <c r="I4" s="21" t="inlineStr">
         <is>
           <t>DE040</t>

</xml_diff>